<commit_message>
feat: fix some issues and import topdown shooter assets
</commit_message>
<xml_diff>
--- a/example/game_06_abyssal_nightfall/bosses.xlsx
+++ b/example/game_06_abyssal_nightfall/bosses.xlsx
@@ -519,7 +519,7 @@
         <v>0.80</v>
       </c>
       <c r="L6" t="str">
-        <v>fx/telegraph/choir_circle.png</v>
+        <v>ui/assets/fx/telegraph/choir_circle.png</v>
       </c>
       <c r="M6" t="str">
         <v>Increases ambient dread by 1 per 20s.</v>
@@ -560,7 +560,7 @@
         <v>1.10</v>
       </c>
       <c r="L7" t="str">
-        <v>fx/telegraph/tidal_lane.png</v>
+        <v>ui/assets/fx/telegraph/tidal_lane.png</v>
       </c>
       <c r="M7" t="str">
         <v>Tidal surges sweep arena edges every 15s.</v>
@@ -601,7 +601,7 @@
         <v>0.95</v>
       </c>
       <c r="L8" t="str">
-        <v>fx/telegraph/beacon_grid.png</v>
+        <v>ui/assets/fx/telegraph/beacon_grid.png</v>
       </c>
       <c r="M8" t="str">
         <v>Reduces sight radius to 65% while active.</v>

</xml_diff>

<commit_message>
gaming (game_06): more assets used
</commit_message>
<xml_diff>
--- a/example/game_06_abyssal_nightfall/bosses.xlsx
+++ b/example/game_06_abyssal_nightfall/bosses.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:M8"/>
+  <dimension ref="A4:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,6 +442,21 @@
       <c r="M4" t="str">
         <v>string</v>
       </c>
+      <c r="N4" t="str">
+        <v>string</v>
+      </c>
+      <c r="O4" t="str">
+        <v>float</v>
+      </c>
+      <c r="P4" t="str">
+        <v>string</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>string</v>
+      </c>
+      <c r="R4" t="str">
+        <v>string</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -483,6 +498,21 @@
       <c r="M5" t="str">
         <v>arenaModifier</v>
       </c>
+      <c r="N5" t="str">
+        <v>sprite</v>
+      </c>
+      <c r="O5" t="str">
+        <v>spriteScale</v>
+      </c>
+      <c r="P5" t="str">
+        <v>deathSprite</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>deathSfx</v>
+      </c>
+      <c r="R5" t="str">
+        <v>themeTrack</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -495,7 +525,7 @@
         <v>0001</v>
       </c>
       <c r="D6" t="str">
-        <v>The Choir of Mouths</v>
+        <v>万口赞歌执政体</v>
       </c>
       <c r="E6" t="str">
         <v>9000</v>
@@ -510,7 +540,7 @@
         <v>20</v>
       </c>
       <c r="I6" t="str">
-        <v>Rotary void beam with hymn barrages</v>
+        <v>旋转虚空光束配合赞歌轰炸</v>
       </c>
       <c r="J6" t="str">
         <v>1.20</v>
@@ -519,10 +549,25 @@
         <v>0.80</v>
       </c>
       <c r="L6" t="str">
-        <v>ui/assets/fx/telegraph/choir_circle.png</v>
+        <v>fx/telegraph/choir_circle.png</v>
       </c>
       <c r="M6" t="str">
-        <v>Increases ambient dread by 1 per 20s.</v>
+        <v>每 20 秒累积 1 层恐惧。</v>
+      </c>
+      <c r="N6" t="str">
+        <v>ui/assets/topdown/top-down-shooter/characters/tank-cannon.png</v>
+      </c>
+      <c r="O6" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="P6" t="str">
+        <v>ui/assets/topdown/top-down-shooter/effects/explosion.png</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>ui/assets/topdown/top-down-shooter/sounds/explosion-3.wav</v>
+      </c>
+      <c r="R6" t="str">
+        <v>ui/assets/topdown/top-down-shooter/music/theme-4.ogg</v>
       </c>
     </row>
     <row r="7">
@@ -536,7 +581,7 @@
         <v>0002</v>
       </c>
       <c r="D7" t="str">
-        <v>Tide Shepherd</v>
+        <v>潮汐引航巨像</v>
       </c>
       <c r="E7" t="str">
         <v>8200</v>
@@ -551,7 +596,7 @@
         <v>18</v>
       </c>
       <c r="I7" t="str">
-        <v>Hook chains pull player into tidal lanes</v>
+        <v>锁链钩拖将玩家拉入潮汐航道</v>
       </c>
       <c r="J7" t="str">
         <v>2.10</v>
@@ -560,10 +605,25 @@
         <v>1.10</v>
       </c>
       <c r="L7" t="str">
-        <v>ui/assets/fx/telegraph/tidal_lane.png</v>
+        <v>fx/telegraph/tidal_lane.png</v>
       </c>
       <c r="M7" t="str">
-        <v>Tidal surges sweep arena edges every 15s.</v>
+        <v>每 15 秒海潮横扫战场边缘。</v>
+      </c>
+      <c r="N7" t="str">
+        <v>ui/assets/topdown/top-down-shooter/characters/tank-base.png</v>
+      </c>
+      <c r="O7" t="str">
+        <v>1.05</v>
+      </c>
+      <c r="P7" t="str">
+        <v>ui/assets/topdown/top-down-shooter/effects/5.png</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>ui/assets/topdown/top-down-shooter/sounds/explosion-2.wav</v>
+      </c>
+      <c r="R7" t="str">
+        <v>ui/assets/topdown/top-down-shooter/music/theme-4.ogg</v>
       </c>
     </row>
     <row r="8">
@@ -577,7 +637,7 @@
         <v>0003</v>
       </c>
       <c r="D8" t="str">
-        <v>Nameless Beacon</v>
+        <v>无名肃光灯塔</v>
       </c>
       <c r="E8" t="str">
         <v>9800</v>
@@ -592,7 +652,7 @@
         <v>24</v>
       </c>
       <c r="I8" t="str">
-        <v>Pillars of surveillance drain sanity</v>
+        <v>监视立柱抽离理智能量</v>
       </c>
       <c r="J8" t="str">
         <v>1.60</v>
@@ -601,15 +661,30 @@
         <v>0.95</v>
       </c>
       <c r="L8" t="str">
-        <v>ui/assets/fx/telegraph/beacon_grid.png</v>
+        <v>fx/telegraph/beacon_grid.png</v>
       </c>
       <c r="M8" t="str">
-        <v>Reduces sight radius to 65% while active.</v>
+        <v>激活时视野压缩至 65%。</v>
+      </c>
+      <c r="N8" t="str">
+        <v>ui/assets/topdown/top-down-shooter/background/door.gif</v>
+      </c>
+      <c r="O8" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="P8" t="str">
+        <v>ui/assets/topdown/top-down-shooter/effects/4.png</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>ui/assets/topdown/top-down-shooter/sounds/explosion-1.wav</v>
+      </c>
+      <c r="R8" t="str">
+        <v>ui/assets/topdown/top-down-shooter/music/theme-4.ogg</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A4:M8"/>
+    <ignoredError numberStoredAsText="1" sqref="A4:R8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>